<commit_message>
attribute 'Art' und 'Träger' hinzugefügt. vorbereitung für implementierung wandler und speicher. kosten*(inst_leistung-untere grenze)
</commit_message>
<xml_diff>
--- a/data/Optimierungsgrößen.xlsx
+++ b/data/Optimierungsgrößen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansisRasanterRaser\Desktop\UNI\000_DA\git\knEBiD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E36CEC8A-57FA-499C-8A5B-5F4D33F4DE8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F006A-11BF-4822-9F76-68C37C095BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -718,7 +718,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,7 +983,7 @@
         <v>30</v>
       </c>
       <c r="D12" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E12" s="1">
         <v>999</v>
@@ -1003,7 +1003,7 @@
         <v>30</v>
       </c>
       <c r="D13" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E13" s="1">
         <v>999</v>
@@ -1027,7 +1027,7 @@
         <v>12368</v>
       </c>
       <c r="E14" s="1">
-        <v>999</v>
+        <v>99999</v>
       </c>
       <c r="F14" s="1">
         <v>999</v>
@@ -1052,7 +1052,7 @@
         <v>9870</v>
       </c>
       <c r="E15" s="1">
-        <v>999</v>
+        <v>9999</v>
       </c>
       <c r="F15" s="1">
         <v>999</v>
@@ -1069,7 +1069,7 @@
         <v>31</v>
       </c>
       <c r="D16" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E16" s="1">
         <v>999</v>
@@ -1089,7 +1089,7 @@
         <v>31</v>
       </c>
       <c r="D17" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E17" s="1">
         <v>999</v>
@@ -1109,7 +1109,7 @@
         <v>30</v>
       </c>
       <c r="D18" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E18" s="1">
         <v>999</v>
@@ -1129,7 +1129,7 @@
         <v>32</v>
       </c>
       <c r="D19" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E19" s="1">
         <v>999</v>
@@ -1149,7 +1149,7 @@
         <v>6</v>
       </c>
       <c r="D20" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E20" s="1">
         <v>999</v>
@@ -1169,7 +1169,7 @@
         <v>29</v>
       </c>
       <c r="D21" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E21" s="1">
         <v>999</v>
@@ -1189,7 +1189,7 @@
         <v>31</v>
       </c>
       <c r="D22" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E22" s="1">
         <v>999</v>
@@ -1209,7 +1209,7 @@
         <v>31</v>
       </c>
       <c r="D23" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E23" s="1">
         <v>999</v>
@@ -1229,7 +1229,7 @@
         <v>29</v>
       </c>
       <c r="D24" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E24" s="1">
         <v>999</v>
@@ -1249,7 +1249,7 @@
         <v>29</v>
       </c>
       <c r="D25" s="1">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1">
         <v>999</v>

</xml_diff>

<commit_message>
strom mit speicher funzt, jedoch noch 'sinnlose' schwankung in be und entladung.
</commit_message>
<xml_diff>
--- a/data/Optimierungsgrößen.xlsx
+++ b/data/Optimierungsgrößen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HansisRasanterRaser\Desktop\UNI\000_DA\git\knEBiD\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506F006A-11BF-4822-9F76-68C37C095BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A475DA3-B18E-4D39-8ED4-8FAE401F4457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
     <author>HansisRasanterRaser</author>
   </authors>
   <commentList>
-    <comment ref="E2" authorId="0" shapeId="0" xr:uid="{6D679327-6FC0-4EDF-8B10-6C4F0C7E874E}">
+    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{6D679327-6FC0-4EDF-8B10-6C4F0C7E874E}">
       <text>
         <r>
           <rPr>
@@ -70,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D5" authorId="0" shapeId="0" xr:uid="{5D612638-672D-4FBD-96AA-CE39C0ABE188}">
+    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{5D612638-672D-4FBD-96AA-CE39C0ABE188}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{52D6F876-3CD2-4EB9-977F-9B9FD472A8C7}">
+    <comment ref="E6" authorId="0" shapeId="0" xr:uid="{52D6F876-3CD2-4EB9-977F-9B9FD472A8C7}">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D10" authorId="0" shapeId="0" xr:uid="{8A1D37A2-13A1-4606-9A45-2559219B3E59}">
+    <comment ref="E10" authorId="0" shapeId="0" xr:uid="{8A1D37A2-13A1-4606-9A45-2559219B3E59}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{3439746B-F33A-45BE-B109-E17AAE67BB7E}">
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{3439746B-F33A-45BE-B109-E17AAE67BB7E}">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Technologie</t>
   </si>
@@ -294,13 +294,88 @@
   </si>
   <si>
     <t>obere Kapagrenze [MWh]</t>
+  </si>
+  <si>
+    <t>Variablenname</t>
+  </si>
+  <si>
+    <t>sp_wae1</t>
+  </si>
+  <si>
+    <t>e_s1</t>
+  </si>
+  <si>
+    <t>e_s2</t>
+  </si>
+  <si>
+    <t>e_s3</t>
+  </si>
+  <si>
+    <t>e_s4</t>
+  </si>
+  <si>
+    <t>e_s5</t>
+  </si>
+  <si>
+    <t>e_s6</t>
+  </si>
+  <si>
+    <t>e_s7</t>
+  </si>
+  <si>
+    <t>e_s8</t>
+  </si>
+  <si>
+    <t>e_wae1</t>
+  </si>
+  <si>
+    <t>e_wae2</t>
+  </si>
+  <si>
+    <t>e_wae3</t>
+  </si>
+  <si>
+    <t>e_wae4</t>
+  </si>
+  <si>
+    <t>sp_s1</t>
+  </si>
+  <si>
+    <t>sp_s2</t>
+  </si>
+  <si>
+    <t>sp_h1</t>
+  </si>
+  <si>
+    <t>sp_h2</t>
+  </si>
+  <si>
+    <t>sp_f1</t>
+  </si>
+  <si>
+    <t>sp_b1</t>
+  </si>
+  <si>
+    <t>w_s_h1</t>
+  </si>
+  <si>
+    <t>w_h_s1</t>
+  </si>
+  <si>
+    <t>w_h_wae1</t>
+  </si>
+  <si>
+    <t>w_s_wae1</t>
+  </si>
+  <si>
+    <t>w_s_wae2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +395,12 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -715,550 +796,739 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="5" width="13.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>38</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>22000</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>99999</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <f>'[1]1'!$B$3*1000</f>
         <v>6439</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <f>[2]Stom!$G$9*1000</f>
         <v>8588</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>6250</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <f>'[1]1'!$F$3*1000</f>
         <v>9172</v>
       </c>
-      <c r="E4">
-        <f>D4+1</f>
+      <c r="F4">
+        <f>E4+1</f>
         <v>9173</v>
       </c>
-      <c r="F4" s="1">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G4" s="1">
+        <v>999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>29</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>29</v>
       </c>
-      <c r="E5">
-        <f>D5+1</f>
+      <c r="F5">
+        <f>E5+1</f>
         <v>30</v>
       </c>
-      <c r="F5" s="1">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G5" s="1">
+        <v>999</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1367</v>
       </c>
-      <c r="E6">
-        <f>D6+1</f>
+      <c r="F6">
+        <f>E6+1</f>
         <v>1368</v>
       </c>
-      <c r="F6" s="1">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G6" s="1">
+        <v>999</v>
+      </c>
+      <c r="H6" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
       <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>29</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <f>'[1]1'!$L$3*1000</f>
         <v>9215</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <f>[2]Stom!$G$13*1000</f>
         <v>70000</v>
       </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>3000</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>36</v>
       </c>
       <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>29</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <f>'[1]1'!$M$3*1000</f>
         <v>63567</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <f>[2]Stom!$G$11*1000</f>
         <v>365900</v>
       </c>
-      <c r="F8" s="1">
+      <c r="G8" s="1">
         <v>1700</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>29</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <f>'[1]1'!$N$3*1000</f>
         <v>100012</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <f>[2]Stom!$G$7*1000</f>
         <v>1045000</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>947</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>4400</v>
       </c>
-      <c r="E10" s="1">
+      <c r="F10" s="1">
         <v>9999</v>
       </c>
-      <c r="F10" s="1">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G10" s="1">
+        <v>999</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>30</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>359</v>
       </c>
-      <c r="E11" s="1">
-        <v>999</v>
-      </c>
       <c r="F11" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G11" s="1">
+        <v>999</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="1">
+      <c r="E12" s="1">
         <v>100</v>
       </c>
-      <c r="E12" s="1">
-        <v>999</v>
-      </c>
       <c r="F12" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G12" s="1">
+        <v>999</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>33</v>
       </c>
       <c r="B13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1">
+      <c r="E13" s="1">
         <v>100</v>
       </c>
-      <c r="E13" s="1">
-        <v>999</v>
-      </c>
       <c r="F13" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G13" s="1">
+        <v>999</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
       <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" t="s">
         <v>14</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>29</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <f>'[1]1'!$D$3*1000</f>
         <v>12368</v>
       </c>
-      <c r="E14" s="1">
+      <c r="F14" s="1">
         <v>99999</v>
       </c>
-      <c r="F14" s="1">
-        <v>999</v>
-      </c>
-      <c r="H14">
+      <c r="G14" s="1">
+        <v>999</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+      <c r="I14">
         <f>'[1]1'!$E$3*1000</f>
         <v>18048</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="1">
+        <v>99999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>29</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <f>'[1]1'!$C$3*1000</f>
         <v>9870</v>
       </c>
-      <c r="E15" s="1">
+      <c r="F15" s="1">
         <v>9999</v>
       </c>
-      <c r="F15" s="1">
-        <v>999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G15" s="1">
+        <v>999</v>
+      </c>
+      <c r="H15" s="1">
+        <v>1</v>
+      </c>
+      <c r="I15" s="1">
+        <v>37000</v>
+      </c>
+      <c r="J15" s="1">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="1">
+      <c r="E16" s="1">
         <v>100</v>
       </c>
-      <c r="E16" s="1">
-        <v>999</v>
-      </c>
       <c r="F16" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="1">
+        <v>999</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" s="1">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="1">
+      <c r="E17" s="1">
         <v>100</v>
       </c>
-      <c r="E17" s="1">
-        <v>999</v>
-      </c>
       <c r="F17" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="1">
+        <v>999</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="J17" s="1">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
         <v>14</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1">
+      <c r="E18" s="1">
         <v>100</v>
       </c>
-      <c r="E18" s="1">
-        <v>999</v>
-      </c>
       <c r="F18" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" s="1">
+        <v>999</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
         <v>14</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="1">
+      <c r="E19" s="1">
         <v>100</v>
       </c>
-      <c r="E19" s="1">
-        <v>999</v>
-      </c>
       <c r="F19" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" s="1">
+        <v>999</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>6</v>
       </c>
-      <c r="D20" s="1">
+      <c r="E20" s="1">
         <v>100</v>
       </c>
-      <c r="E20" s="1">
-        <v>999</v>
-      </c>
       <c r="F20" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" s="1">
+        <v>999</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="J20" s="1">
+        <v>99999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
       <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>22</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="1">
+      <c r="E21" s="1">
         <v>100</v>
       </c>
-      <c r="E21" s="1">
-        <v>999</v>
-      </c>
       <c r="F21" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" s="1">
+        <v>999</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>24</v>
       </c>
       <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" t="s">
         <v>22</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>31</v>
       </c>
-      <c r="D22" s="1">
+      <c r="E22" s="1">
         <v>100</v>
       </c>
-      <c r="E22" s="1">
-        <v>999</v>
-      </c>
       <c r="F22" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" s="1">
+        <v>999</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>25</v>
       </c>
       <c r="B23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
         <v>22</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>31</v>
       </c>
-      <c r="D23" s="1">
+      <c r="E23" s="1">
         <v>100</v>
       </c>
-      <c r="E23" s="1">
-        <v>999</v>
-      </c>
       <c r="F23" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" s="1">
+        <v>999</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
       <c r="B24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" t="s">
         <v>22</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="1">
+      <c r="E24" s="1">
         <v>100</v>
       </c>
-      <c r="E24" s="1">
-        <v>999</v>
-      </c>
       <c r="F24" s="1">
         <v>999</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>999</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
       <c r="B25" t="s">
+        <v>64</v>
+      </c>
+      <c r="C25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="1">
+      <c r="E25" s="1">
         <v>100</v>
       </c>
-      <c r="E25" s="1">
-        <v>999</v>
-      </c>
       <c r="F25" s="1">
         <v>999</v>
       </c>
+      <c r="G25" s="1">
+        <v>999</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>